<commit_message>
update scripts and excels
</commit_message>
<xml_diff>
--- a/Defaults/defaults.xlsx
+++ b/Defaults/defaults.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="170">
   <si>
     <t xml:space="preserve">Optimizers</t>
   </si>
@@ -36,15 +36,24 @@
     <t xml:space="preserve">SGD</t>
   </si>
   <si>
+    <t xml:space="preserve">clipnorm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lample et al</t>
   </si>
   <si>
+    <t xml:space="preserve">vs</t>
+  </si>
+  <si>
     <t xml:space="preserve">Keras</t>
   </si>
   <si>
     <t xml:space="preserve">Zhilin Yang</t>
   </si>
   <si>
+    <t xml:space="preserve">clipvalue</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://cs231n.github.io/neural-networks-3/#ada</t>
   </si>
   <si>
@@ -58,6 +67,12 @@
   </si>
   <si>
     <t xml:space="preserve">NO FUCKING CLUE!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categorical_crossentropy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keras_contrib</t>
   </si>
   <si>
     <t xml:space="preserve">Trainable embedding</t>
@@ -617,8 +632,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -671,15 +690,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>54000</xdr:colOff>
+      <xdr:colOff>12600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>27360</xdr:rowOff>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>762480</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>54360</xdr:rowOff>
+      <xdr:colOff>569160</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>108360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -692,8 +711,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3254400" y="189720"/>
-          <a:ext cx="3108600" cy="1490040"/>
+          <a:off x="2412720" y="171720"/>
+          <a:ext cx="2356920" cy="1399680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -710,13 +729,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:rowOff>44280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>758520</xdr:colOff>
+      <xdr:colOff>582120</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>104760</xdr:rowOff>
+      <xdr:rowOff>97560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -729,8 +748,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7200720" y="200160"/>
-          <a:ext cx="3958920" cy="229680"/>
+          <a:off x="5400360" y="206640"/>
+          <a:ext cx="2982600" cy="216000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -750,10 +769,10 @@
       <xdr:rowOff>39240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>749880</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>149040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>102960</xdr:rowOff>
+      <xdr:rowOff>102240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -766,45 +785,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7236720" y="1989720"/>
-          <a:ext cx="3914280" cy="226440"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>44640</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>750240</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 4" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3245040" y="2806920"/>
-          <a:ext cx="5506200" cy="576360"/>
+          <a:off x="5436360" y="1989720"/>
+          <a:ext cx="3113640" cy="225720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -825,23 +807,23 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
+      <xdr:colOff>365040</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>32040</xdr:rowOff>
+      <xdr:rowOff>31320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 6" descr=""/>
+        <xdr:cNvPr id="3" name="Image 6" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
+        <a:blip r:embed="rId4"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12054960" y="253800"/>
-          <a:ext cx="1912320" cy="590760"/>
+          <a:off x="9054720" y="253800"/>
+          <a:ext cx="1511280" cy="590040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -862,13 +844,50 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>392760</xdr:colOff>
+      <xdr:colOff>392040</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>151200</xdr:rowOff>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Image 7" descr=""/>
+        <xdr:cNvPr id="4" name="Image 7" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId5"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9063720" y="852840"/>
+          <a:ext cx="1529280" cy="760680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>4320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>136080</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>64800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 13" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -877,8 +896,45 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12063960" y="852840"/>
-          <a:ext cx="1930320" cy="761400"/>
+          <a:off x="3600360" y="2442600"/>
+          <a:ext cx="3736440" cy="385560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>44640</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>43560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>149400</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>131400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId7"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2444760" y="3132000"/>
+          <a:ext cx="4305240" cy="575640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -894,28 +950,28 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>35640</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>28800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>535680</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:colOff>534960</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>137880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Image 8" descr=""/>
+        <xdr:cNvPr id="7" name="Image 8" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId7"/>
+        <a:blip r:embed="rId8"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3236040" y="6206040"/>
-          <a:ext cx="2100240" cy="1085040"/>
+          <a:off x="2435760" y="6531120"/>
+          <a:ext cx="1699560" cy="1084320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -931,28 +987,28 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>44640</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>7920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>732240</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>131400</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>141480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Image 9" descr=""/>
+        <xdr:cNvPr id="8" name="Image 9" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId8"/>
+        <a:blip r:embed="rId9"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3245040" y="7485480"/>
-          <a:ext cx="2287800" cy="2085120"/>
+          <a:off x="2444760" y="7810560"/>
+          <a:ext cx="1887120" cy="2084400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -968,28 +1024,28 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>57600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>740880</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>75600</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>140400</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 5" descr=""/>
+        <xdr:cNvPr id="9" name="Image 5" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId9"/>
+        <a:blip r:embed="rId10"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3200400" y="9811080"/>
-          <a:ext cx="3941280" cy="343080"/>
+          <a:off x="2400120" y="10136160"/>
+          <a:ext cx="3140640" cy="342360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1005,28 +1061,28 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>36000</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>32040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>527040</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>53640</xdr:rowOff>
+      <xdr:colOff>526320</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>52920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Image 10" descr=""/>
+        <xdr:cNvPr id="10" name="Image 10" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId10"/>
+        <a:blip r:embed="rId11"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3236400" y="3933360"/>
-          <a:ext cx="2091240" cy="834480"/>
+          <a:off x="2436120" y="4258440"/>
+          <a:ext cx="1690560" cy="833760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1042,28 +1098,28 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>312840</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>15840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>723600</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>90360</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>122760</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>89640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Image 11" descr=""/>
+        <xdr:cNvPr id="11" name="Image 11" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId11"/>
+        <a:blip r:embed="rId12"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8313840" y="3917160"/>
-          <a:ext cx="3611160" cy="887400"/>
+          <a:off x="6313320" y="4242240"/>
+          <a:ext cx="2810520" cy="886680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1079,28 +1135,65 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>27000</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>16560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>535680</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:colOff>534960</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>131400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Image 12" descr=""/>
+        <xdr:cNvPr id="12" name="Image 12" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId12"/>
+        <a:blip r:embed="rId13"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4027320" y="10908000"/>
-          <a:ext cx="2108880" cy="765720"/>
+          <a:off x="3027240" y="11233080"/>
+          <a:ext cx="1708200" cy="765000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>107280</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>36000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>36000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>129240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Image 14" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId14"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12108600" y="198360"/>
+          <a:ext cx="4729320" cy="3182040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1120,252 +1213,269 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:O70"/>
+  <dimension ref="B2:T72"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T6" activeCellId="0" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="O2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="T2" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O3" s="0" t="s">
-        <v>4</v>
+      <c r="O3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>6</v>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D12" s="0" t="s">
-        <v>7</v>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I13" s="0" t="s">
-        <v>6</v>
+      <c r="I13" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="0" t="n">
+      <c r="B14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="n">
         <v>0.001</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="0" t="n">
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="1" t="n">
         <v>0.01</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="1" t="n">
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="1" t="n">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="0" t="n">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="I25" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D26" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
+      <c r="I27" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I30" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="J30" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="0" t="s">
-        <v>19</v>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E35" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="0" t="n">
+      <c r="E37" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="E37" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="0" t="s">
+      <c r="E39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D61" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="K61" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D62" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="K62" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D65" s="0" t="s">
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F65" s="0" t="s">
+      <c r="D41" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H65" s="0" t="s">
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D42" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I65" s="0" t="s">
+      <c r="D49" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D50" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K65" s="0" t="s">
+      <c r="D63" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B67" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D66" s="0" t="s">
+      <c r="D67" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="F67" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D69" s="0" t="s">
-        <v>36</v>
+      <c r="D68" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D70" s="0" t="s">
-        <v>37</v>
+      <c r="B70" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D71" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D72" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="I26:J29"/>
+    <mergeCell ref="I28:J31"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -1391,572 +1501,572 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="s">
-        <v>38</v>
+      <c r="B2" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3" t="s">
-        <v>39</v>
+      <c r="B4" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3" t="s">
-        <v>40</v>
+      <c r="B6" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="3" t="s">
-        <v>41</v>
+      <c r="B7" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="s">
-        <v>42</v>
+      <c r="B8" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="3" t="s">
-        <v>43</v>
+      <c r="B9" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5" t="s">
-        <v>44</v>
+      <c r="B10" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="3" t="s">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="5" t="s">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="3" t="s">
-        <v>79</v>
+      <c r="B50" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="3" t="s">
-        <v>80</v>
+      <c r="B51" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="3" t="s">
-        <v>81</v>
+      <c r="B52" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="3" t="s">
-        <v>82</v>
+      <c r="B53" s="4" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="3" t="s">
-        <v>83</v>
+      <c r="B54" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="3" t="s">
-        <v>81</v>
+      <c r="B55" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="3" t="s">
-        <v>84</v>
+      <c r="B56" s="4" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="3" t="s">
-        <v>85</v>
+      <c r="B57" s="4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="3" t="s">
-        <v>81</v>
+      <c r="B58" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="3" t="s">
-        <v>87</v>
+      <c r="B61" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="3" t="s">
-        <v>88</v>
+      <c r="B62" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="3" t="s">
-        <v>89</v>
+      <c r="B63" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="3" t="s">
-        <v>90</v>
+      <c r="B64" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="3" t="s">
-        <v>91</v>
+      <c r="B65" s="4" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="3" t="s">
-        <v>92</v>
+      <c r="B66" s="4" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="3" t="s">
-        <v>93</v>
+      <c r="B67" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="3" t="s">
-        <v>94</v>
+      <c r="B68" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="3" t="s">
-        <v>95</v>
+      <c r="B69" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="3" t="s">
-        <v>93</v>
+      <c r="B70" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="3" t="s">
-        <v>96</v>
+      <c r="B71" s="4" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B75" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B76" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B77" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B79" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="3" t="s">
-        <v>100</v>
+      <c r="B81" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="3" t="s">
-        <v>102</v>
+      <c r="B82" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="3" t="s">
-        <v>103</v>
+      <c r="B83" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="3" t="s">
-        <v>100</v>
+      <c r="B84" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="3" t="s">
-        <v>104</v>
+      <c r="B85" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="3" t="s">
-        <v>100</v>
+      <c r="B86" s="4" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="3" t="s">
-        <v>105</v>
+      <c r="B87" s="4" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="3" t="s">
-        <v>106</v>
+      <c r="B88" s="4" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="3" t="s">
-        <v>107</v>
+      <c r="B89" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="3" t="s">
-        <v>108</v>
+      <c r="B90" s="4" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="3" t="s">
-        <v>109</v>
+      <c r="B91" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="3" t="s">
-        <v>110</v>
+      <c r="B92" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="3" t="s">
-        <v>111</v>
+      <c r="B94" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="7"/>
-      <c r="C95" s="3" t="s">
-        <v>112</v>
+      <c r="B95" s="8"/>
+      <c r="C95" s="4" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="7"/>
-      <c r="C96" s="3" t="s">
-        <v>113</v>
+      <c r="B96" s="8"/>
+      <c r="C96" s="4" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="7"/>
-      <c r="C97" s="3" t="s">
-        <v>114</v>
+      <c r="B97" s="8"/>
+      <c r="C97" s="4" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="7"/>
-      <c r="C98" s="3" t="s">
-        <v>115</v>
+      <c r="B98" s="8"/>
+      <c r="C98" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="7"/>
-      <c r="C99" s="3" t="s">
-        <v>116</v>
+      <c r="B99" s="8"/>
+      <c r="C99" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="7"/>
-      <c r="C100" s="3" t="s">
-        <v>117</v>
+      <c r="B100" s="8"/>
+      <c r="C100" s="4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="7"/>
-      <c r="C101" s="3" t="s">
-        <v>118</v>
+      <c r="B101" s="8"/>
+      <c r="C101" s="4" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="7"/>
-      <c r="C102" s="3" t="s">
-        <v>119</v>
+      <c r="B102" s="8"/>
+      <c r="C102" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="7"/>
-      <c r="C103" s="3" t="s">
-        <v>120</v>
+      <c r="B103" s="8"/>
+      <c r="C103" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="7"/>
-      <c r="C104" s="3" t="s">
-        <v>121</v>
+      <c r="B104" s="8"/>
+      <c r="C104" s="4" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="7"/>
-      <c r="C105" s="3" t="s">
-        <v>122</v>
+      <c r="B105" s="8"/>
+      <c r="C105" s="4" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="7"/>
-      <c r="C106" s="3" t="s">
-        <v>123</v>
+      <c r="B106" s="8"/>
+      <c r="C106" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="7"/>
-      <c r="C107" s="3" t="s">
-        <v>124</v>
+      <c r="B107" s="8"/>
+      <c r="C107" s="4" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="7"/>
-      <c r="C108" s="3" t="s">
-        <v>125</v>
+      <c r="B108" s="8"/>
+      <c r="C108" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="7"/>
-      <c r="C109" s="3" t="s">
-        <v>126</v>
+      <c r="B109" s="8"/>
+      <c r="C109" s="4" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="7"/>
-      <c r="C110" s="3" t="s">
-        <v>127</v>
+      <c r="B110" s="8"/>
+      <c r="C110" s="4" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="7"/>
-      <c r="C111" s="3" t="s">
-        <v>128</v>
+      <c r="B111" s="8"/>
+      <c r="C111" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="7"/>
-      <c r="C112" s="3" t="s">
-        <v>129</v>
+      <c r="B112" s="8"/>
+      <c r="C112" s="4" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="7"/>
-      <c r="C113" s="3" t="s">
-        <v>130</v>
+      <c r="B113" s="8"/>
+      <c r="C113" s="4" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="7"/>
-      <c r="C114" s="3" t="s">
-        <v>131</v>
+      <c r="B114" s="8"/>
+      <c r="C114" s="4" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="4" t="s">
-        <v>14</v>
+      <c r="B116" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1997,190 +2107,190 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="4" t="s">
-        <v>132</v>
+      <c r="B2" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="3" t="s">
-        <v>133</v>
+      <c r="B4" s="4" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="3" t="s">
-        <v>40</v>
+      <c r="B6" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5" t="s">
-        <v>134</v>
+      <c r="B7" s="6" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5" t="s">
-        <v>135</v>
+      <c r="B8" s="6" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="3" t="s">
-        <v>136</v>
+      <c r="B9" s="4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="3" t="s">
-        <v>137</v>
+      <c r="B10" s="4" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="3" t="s">
-        <v>138</v>
+      <c r="B11" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="3" t="s">
-        <v>139</v>
+      <c r="B12" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="3" t="s">
-        <v>140</v>
+      <c r="B13" s="4" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="3" t="s">
-        <v>141</v>
+      <c r="B14" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="4" t="s">
-        <v>142</v>
+      <c r="B16" s="5" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="3" t="s">
-        <v>143</v>
+      <c r="B18" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="3" t="s">
-        <v>40</v>
+      <c r="B20" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="3" t="s">
-        <v>144</v>
+      <c r="B21" s="4" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="3" t="s">
-        <v>145</v>
+      <c r="B22" s="4" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="3" t="s">
-        <v>146</v>
+      <c r="B23" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="3" t="s">
-        <v>147</v>
+      <c r="B24" s="4" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="3" t="s">
-        <v>148</v>
+      <c r="B25" s="4" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="5" t="s">
-        <v>149</v>
+      <c r="B26" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="3" t="s">
-        <v>150</v>
+      <c r="B27" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="3" t="s">
-        <v>151</v>
+      <c r="B28" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="3" t="s">
-        <v>152</v>
+      <c r="B29" s="4" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="3" t="s">
-        <v>153</v>
+      <c r="B30" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="3" t="s">
-        <v>154</v>
+      <c r="B31" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="3" t="s">
-        <v>155</v>
+      <c r="B32" s="4" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="3" t="s">
-        <v>156</v>
+      <c r="B33" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="3" t="s">
-        <v>157</v>
+      <c r="B34" s="4" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="4" t="s">
-        <v>158</v>
+      <c r="B36" s="5" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="3" t="s">
-        <v>159</v>
+      <c r="B38" s="4" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="8"/>
+      <c r="B39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="3" t="s">
-        <v>40</v>
+      <c r="B40" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="3" t="s">
-        <v>160</v>
+      <c r="B41" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="3" t="s">
-        <v>161</v>
+      <c r="B42" s="4" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="3" t="s">
-        <v>162</v>
+      <c r="B43" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="3" t="s">
-        <v>163</v>
+      <c r="B44" s="4" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="3" t="s">
-        <v>164</v>
+      <c r="B45" s="4" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>